<commit_message>
Ran 1st analysis in Python.
</commit_message>
<xml_diff>
--- a/excel/excel_analysis.xlsx
+++ b/excel/excel_analysis.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="21480" windowHeight="10035"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="21480" windowHeight="10035" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="data" sheetId="1" r:id="rId2"/>
     <sheet name="Lookup" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
@@ -16,7 +16,7 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="31" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -18134,7 +18134,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C32" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -18569,7 +18569,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
@@ -19167,7 +19167,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N892"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>

</xml_diff>